<commit_message>
EPBDS-10426 EPBDS-10554 Do warning instead of error for dispatched methods with aliases in arguments
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10554_ConflictsMethodParams.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10554_ConflictsMethodParams.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\Bugz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A486B34-0139-4D28-8385-B54DCA45FE4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FCF3DA-EF75-463C-88FB-8815E90459C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="990" windowWidth="23895" windowHeight="13470" xr2:uid="{7E830EE8-BA71-43AB-AAAE-EBFB2EE13E74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7E830EE8-BA71-43AB-AAAE-EBFB2EE13E74}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Names" sheetId="1" r:id="rId1"/>
+    <sheet name="Types" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
-  <si>
-    <t>Spreadsheet SpreadsheetResult mySpr(Integer myParam, Double anotherParam)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>Steps</t>
   </si>
@@ -44,9 +46,6 @@
     <t>Step1</t>
   </si>
   <si>
-    <t>Step2</t>
-  </si>
-  <si>
     <t>properties</t>
   </si>
   <si>
@@ -59,21 +58,105 @@
     <t>KY,LA</t>
   </si>
   <si>
-    <t>Spreadsheet SpreadsheetResult mySpr(Integer helloParam, Double ololoParam)</t>
+    <t>Spreadsheet Integer calc(String input)</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Spreadsheet Integer calc(Vocabular input)</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>Datatype Vocabular &lt;String&gt;</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Test calc</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>_context_.usState</t>
+  </si>
+  <si>
+    <t>_res_</t>
+  </si>
+  <si>
+    <t>_error_</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>Object 'DA' is outside of valid domain 'Vocabular'. Valid values: [NY, AL]</t>
+  </si>
+  <si>
+    <t>Test mySpr</t>
+  </si>
+  <si>
+    <t>myParam</t>
+  </si>
+  <si>
+    <t>anotherParam</t>
+  </si>
+  <si>
+    <t>Input 2</t>
+  </si>
+  <si>
+    <t>Spreadsheet Integer mySpr(Integer myParam, Double anotherParam)</t>
+  </si>
+  <si>
+    <t>Spreadsheet Integer mySpr(Integer helloParam, Double ololoParam)</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>KY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -94,23 +177,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{0621B71E-20E2-493C-9D20-AF164C8331F3}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -126,9 +209,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -166,7 +249,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -272,7 +355,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -422,127 +505,337 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC3E852-4079-4AA1-818B-B80D8821F40C}">
-  <dimension ref="B13:F24"/>
+  <dimension ref="B3:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="E13"/>
-    </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D15" t="s" s="0">
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="D11" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D16" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E16" t="n" s="0">
+      <c r="C12" s="5">
+        <v>2</v>
+      </c>
+      <c r="D12" s="6">
         <f>6</f>
-        <v>6.0</v>
-      </c>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17">
-      <c r="D17" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E17" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18">
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="0"/>
-      <c r="D20" s="0"/>
-    </row>
-    <row r="21">
-      <c r="B21" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="D21" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="s" s="0">
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18">
         <v>1</v>
       </c>
-      <c r="C22" s="0" t="s">
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19">
         <v>2</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C23" t="n" s="0">
-        <f>6</f>
-        <v>6.0</v>
-      </c>
-      <c r="D23" s="8" t="n">
-        <f>6</f>
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C24" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="D24" s="9" t="n">
-        <v>7.0</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
+  <mergeCells count="6">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB60D17-EFE2-4B7C-A1B0-D2B67D56CAFC}">
+  <dimension ref="B3:E28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Backed out changeset: cf7e0edac6b3
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10554_ConflictsMethodParams.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10554_ConflictsMethodParams.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\Bugz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A486B34-0139-4D28-8385-B54DCA45FE4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FCF3DA-EF75-463C-88FB-8815E90459C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="990" windowWidth="23895" windowHeight="13470" xr2:uid="{7E830EE8-BA71-43AB-AAAE-EBFB2EE13E74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7E830EE8-BA71-43AB-AAAE-EBFB2EE13E74}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Names" sheetId="1" r:id="rId1"/>
+    <sheet name="Types" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
-  <si>
-    <t>Spreadsheet SpreadsheetResult mySpr(Integer myParam, Double anotherParam)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>Steps</t>
   </si>
@@ -44,9 +46,6 @@
     <t>Step1</t>
   </si>
   <si>
-    <t>Step2</t>
-  </si>
-  <si>
     <t>properties</t>
   </si>
   <si>
@@ -59,21 +58,105 @@
     <t>KY,LA</t>
   </si>
   <si>
-    <t>Spreadsheet SpreadsheetResult mySpr(Integer helloParam, Double ololoParam)</t>
+    <t>Spreadsheet Integer calc(String input)</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Spreadsheet Integer calc(Vocabular input)</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>Datatype Vocabular &lt;String&gt;</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Test calc</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>_context_.usState</t>
+  </si>
+  <si>
+    <t>_res_</t>
+  </si>
+  <si>
+    <t>_error_</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>Object 'DA' is outside of valid domain 'Vocabular'. Valid values: [NY, AL]</t>
+  </si>
+  <si>
+    <t>Test mySpr</t>
+  </si>
+  <si>
+    <t>myParam</t>
+  </si>
+  <si>
+    <t>anotherParam</t>
+  </si>
+  <si>
+    <t>Input 2</t>
+  </si>
+  <si>
+    <t>Spreadsheet Integer mySpr(Integer myParam, Double anotherParam)</t>
+  </si>
+  <si>
+    <t>Spreadsheet Integer mySpr(Integer helloParam, Double ololoParam)</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>KY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -94,23 +177,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{0621B71E-20E2-493C-9D20-AF164C8331F3}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -126,9 +209,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -166,7 +249,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -272,7 +355,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -422,127 +505,337 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC3E852-4079-4AA1-818B-B80D8821F40C}">
-  <dimension ref="B13:F24"/>
+  <dimension ref="B3:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="E13"/>
-    </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D15" t="s" s="0">
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="D11" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D16" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E16" t="n" s="0">
+      <c r="C12" s="5">
+        <v>2</v>
+      </c>
+      <c r="D12" s="6">
         <f>6</f>
-        <v>6.0</v>
-      </c>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17">
-      <c r="D17" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E17" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18">
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="0"/>
-      <c r="D20" s="0"/>
-    </row>
-    <row r="21">
-      <c r="B21" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="D21" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="s" s="0">
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18">
         <v>1</v>
       </c>
-      <c r="C22" s="0" t="s">
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19">
         <v>2</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C23" t="n" s="0">
-        <f>6</f>
-        <v>6.0</v>
-      </c>
-      <c r="D23" s="8" t="n">
-        <f>6</f>
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C24" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="D24" s="9" t="n">
-        <v>7.0</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
+  <mergeCells count="6">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB60D17-EFE2-4B7C-A1B0-D2B67D56CAFC}">
+  <dimension ref="B3:E28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>